<commit_message>
Running nginx server on port 3000 and minor schema changes
</commit_message>
<xml_diff>
--- a/rspack-ui/test/test-spreadsheet.xlsx
+++ b/rspack-ui/test/test-spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninja/Documents/Projects/PHAC/safe-inputs/rspack-ui/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CBF328-1343-E04C-8621-8E136A966CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33B2F9E-5179-8D4D-91BB-4B858F99BF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{E1007137-725D-984E-B083-456ECCE3345A}" name="test" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/ninja/Documents/Projects/PHAC/safe-inputs/rspack-ui/src/schema/test" tab="0" comma="1">
+    <textPr sourceFile="/Users/ninja/Documents/Projects/PHAC/safe-inputs/rspack-ui/src/schema/test" tab="0" comma="1">
       <textFields count="12">
         <textField/>
         <textField/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="110">
   <si>
     <t>M</t>
   </si>
@@ -86,9 +86,6 @@
     <t>treatingPhysician</t>
   </si>
   <si>
-    <t>medications</t>
-  </si>
-  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Dr. Smith</t>
   </si>
   <si>
-    <t>Medicine A, Medicine B</t>
-  </si>
-  <si>
     <t>Jane Smith</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>Dr. Garcia</t>
   </si>
   <si>
-    <t>Medicine D, Medicine E</t>
-  </si>
-  <si>
     <t>Maria Hernandez</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
     <t>Dr. Martinez</t>
   </si>
   <si>
-    <t>Medicine G, Medicine H</t>
-  </si>
-  <si>
     <t>Sarah Liu</t>
   </si>
   <si>
@@ -185,9 +173,6 @@
     <t>Dr. Adams</t>
   </si>
   <si>
-    <t>Medicine J, Medicine K</t>
-  </si>
-  <si>
     <t>Ava Martinez</t>
   </si>
   <si>
@@ -287,9 +272,6 @@
     <t>Dr. Hernandez</t>
   </si>
   <si>
-    <t>Medicine M, Medicine N</t>
-  </si>
-  <si>
     <t>Isabella Nguyen</t>
   </si>
   <si>
@@ -375,6 +357,30 @@
   </si>
   <si>
     <t>2023 June 02</t>
+  </si>
+  <si>
+    <t>Medicine A</t>
+  </si>
+  <si>
+    <t>Medicine  E</t>
+  </si>
+  <si>
+    <t>Medicine H</t>
+  </si>
+  <si>
+    <t>Medicine J</t>
+  </si>
+  <si>
+    <t>Medicine N</t>
+  </si>
+  <si>
+    <t>medication</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -745,7 +751,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -783,19 +789,19 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -803,34 +809,34 @@
         <v>1001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>-1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="b">
-        <v>1</v>
+      <c r="G2" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -838,7 +844,7 @@
         <v>1002</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>45</v>
@@ -847,16 +853,16 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -866,34 +872,34 @@
         <v>1003</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1">
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -901,28 +907,28 @@
         <v>1004</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1">
         <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -932,7 +938,7 @@
         <v>1005</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1">
         <v>40</v>
@@ -941,22 +947,22 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="b">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -964,28 +970,28 @@
         <v>1006</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1">
         <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="1" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -995,34 +1001,34 @@
         <v>1007</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
         <v>55</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="1" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1030,25 +1036,25 @@
         <v>1008</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
         <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="1" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1058,34 +1064,34 @@
         <v>1009</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1">
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1" t="b">
-        <v>1</v>
+      <c r="G10" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1093,28 +1099,28 @@
         <v>1010</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1">
         <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="1" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1124,34 +1130,34 @@
         <v>1011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1">
         <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="1" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1159,25 +1165,25 @@
         <v>1012</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1">
         <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="1" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1187,34 +1193,34 @@
         <v>1013</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1">
         <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="1" t="b">
-        <v>1</v>
+      <c r="G14" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1222,25 +1228,25 @@
         <v>1014</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1">
         <v>55</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="1" t="b">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1250,34 +1256,34 @@
         <v>1015</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1">
         <v>47</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="1" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1285,34 +1291,34 @@
         <v>1016</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1">
         <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="1" t="b">
-        <v>1</v>
+      <c r="G17" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1320,28 +1326,28 @@
         <v>1017</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1">
         <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="1" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1351,25 +1357,25 @@
         <v>1018</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1">
         <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="1" t="b">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1379,34 +1385,34 @@
         <v>1019</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1">
         <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="1" t="b">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1414,28 +1420,28 @@
         <v>1020</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1">
         <v>37</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="1" t="b">
-        <v>1</v>
+      <c r="G21" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>

</xml_diff>